<commit_message>
update code xử lý
</commit_message>
<xml_diff>
--- a/CheckinManagementSystem/Word/formImport.xlsx
+++ b/CheckinManagementSystem/Word/formImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\C#\check-in-out-software\CheckinManagementSystem\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921277B0-2BFC-4D8B-ABE4-62E903037D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A62B4DA-69B6-45F4-ADAA-422D4AF9CC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7680" yWindow="4476" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>STT</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Phòng kinh doanh</t>
   </si>
   <si>
-    <t>NS4</t>
-  </si>
-  <si>
     <t>Phòng nhân sự</t>
   </si>
   <si>
@@ -59,6 +56,18 @@
   </si>
   <si>
     <t>NS7</t>
+  </si>
+  <si>
+    <t>NS71</t>
+  </si>
+  <si>
+    <t>NS42</t>
+  </si>
+  <si>
+    <t>NS15</t>
+  </si>
+  <si>
+    <t>NS61</t>
   </si>
 </sst>
 </file>
@@ -499,7 +508,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -511,7 +520,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -534,10 +543,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -569,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>2</v>
@@ -583,10 +592,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>4</v>
@@ -597,10 +606,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>4</v>
@@ -611,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13">

</xml_diff>